<commit_message>
Node Js: Se realiza el ajuste de extracion de datos para provedor estandar y se crea el xlsx de manera local
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,15 @@
       <c r="E1" t="str">
         <v>MAC CENTER BOGOTA CITY U</v>
       </c>
+      <c r="F1" t="str">
+        <v>661-17165</v>
+      </c>
+      <c r="G1" t="str">
+        <v>AIRPODS PRO 1ST GEN, RIGHT, CI/AR</v>
+      </c>
+      <c r="H1" t="str">
+        <v>349.411,50</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -435,6 +444,15 @@
       <c r="E2" t="str">
         <v>MAC CENTER COLOMBIA MULTIPLAZA</v>
       </c>
+      <c r="F2" t="str">
+        <v>Z661-13579</v>
+      </c>
+      <c r="G2" t="str">
+        <v>SPACE GRAY, 128GB, IPAD 7TH GEN, WI-FI, INT</v>
+      </c>
+      <c r="H2" t="str">
+        <v>1.009.873,75</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -452,6 +470,15 @@
       <c r="E3" t="str">
         <v>MAC CENTER PARQUE LA 93</v>
       </c>
+      <c r="F3" t="str">
+        <v>LL661-42726</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Display, iPhone 16 Pro, USA</v>
+      </c>
+      <c r="H3" t="str">
+        <v>1.380.293,95</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -469,6 +496,15 @@
       <c r="E4" t="str">
         <v>MAC CENTER ANDINO BOGOTA</v>
       </c>
+      <c r="F4" t="str">
+        <v>923-03869</v>
+      </c>
+      <c r="G4" t="str">
+        <v>AIRPODS PRO 1ST GEN, EAR TIPS, MEDIUM</v>
+      </c>
+      <c r="H4" t="str">
+        <v>15.462,00</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -486,6 +522,15 @@
       <c r="E5" t="str">
         <v>MAC CENTER PARQUE LA 93</v>
       </c>
+      <c r="F5" t="str">
+        <v>923-04957</v>
+      </c>
+      <c r="G5" t="str">
+        <v>BLACK, AIRPODS MAX, LEFT, EAR CUSHION</v>
+      </c>
+      <c r="H5" t="str">
+        <v>142.941,60</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -503,6 +548,15 @@
       <c r="E6" t="str">
         <v>MAC CENTER TESORO MEDELLIN</v>
       </c>
+      <c r="F6" t="str">
+        <v>923-03869</v>
+      </c>
+      <c r="G6" t="str">
+        <v>AIRPODS PRO 1ST GEN, EAR TIPS, MEDIUM</v>
+      </c>
+      <c r="H6" t="str">
+        <v>15.462,00</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -520,6 +574,15 @@
       <c r="E7" t="str">
         <v>MAC CENTER PARQUE LA 93</v>
       </c>
+      <c r="F7" t="str">
+        <v>923-03869</v>
+      </c>
+      <c r="G7" t="str">
+        <v>AIRPODS PRO 1ST GEN, EAR TIPS, MEDIUM</v>
+      </c>
+      <c r="H7" t="str">
+        <v>15.462,00</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -537,10 +600,19 @@
       <c r="E8" t="str">
         <v>MAC CENTER PARQUE LA 93</v>
       </c>
+      <c r="F8" t="str">
+        <v>923-03869</v>
+      </c>
+      <c r="G8" t="str">
+        <v>AIRPODS PRO 1ST GEN, EAR TIPS, MEDIUM</v>
+      </c>
+      <c r="H8" t="str">
+        <v>15.462,00</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>